<commit_message>
Added app function for overall program, needs adjustment to eliminate errors
</commit_message>
<xml_diff>
--- a/Ace_Ventura.xlsx
+++ b/Ace_Ventura.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,6 +440,32 @@
           <t>Director</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>rekisela@uw.edu</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Jim Kisela</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ace Ventura</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -461,6 +487,62 @@
           <t>Editor</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>rekisela@uw.edu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Napoleon Bonaparte</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ace Ventura</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Blazing Saddles</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Editor</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Special Effects</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Camera Operator</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -489,6 +571,62 @@
           <t>Camera Operator</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>rekisela@uw.edu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ann Kisela</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ace Ventura</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Blazing Saddles</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Camera Operator</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Assistant Director</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Production Assistant</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -529,6 +667,69 @@
       <c r="A15" t="inlineStr">
         <is>
           <t>Script Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Production Assistant</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>rekisela@uw.edu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Fake Name 3</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ace Ventura</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Blazing Saddles</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Production Assistant</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Assistant Camera Operator</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Art Department</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Role</t>
         </is>
       </c>
     </row>

</xml_diff>